<commit_message>
updating leaky current integration
</commit_message>
<xml_diff>
--- a/reusable_module/benchmark.xlsx
+++ b/reusable_module/benchmark.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Num Neruons</t>
   </si>
@@ -79,6 +80,33 @@
   <si>
     <t>secs</t>
   </si>
+  <si>
+    <t>1 min 9 secs</t>
+  </si>
+  <si>
+    <t>1 min 10 secs</t>
+  </si>
+  <si>
+    <t>1 min 7 secs</t>
+  </si>
+  <si>
+    <t>2 min 21 secs</t>
+  </si>
+  <si>
+    <t>2 min 13 secs</t>
+  </si>
+  <si>
+    <t>2 min 29 secs</t>
+  </si>
+  <si>
+    <t>5 min 11 secs</t>
+  </si>
+  <si>
+    <t>5 min 8 secs</t>
+  </si>
+  <si>
+    <t>5 min 34 secs</t>
+  </si>
 </sst>
 </file>
 
@@ -124,12 +152,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,7 +257,7 @@
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -237,8 +266,10 @@
             <c:v>125 neurons</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -319,18 +350,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>181.0</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>286.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -339,8 +370,10 @@
             <c:v>250 neurons</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -421,18 +454,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>473.0</c:v>
+                  <c:v>141.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>683.0</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1380.0</c:v>
+                  <c:v>149.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -441,8 +474,10 @@
             <c:v>500 neurons</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -523,18 +558,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3770.0</c:v>
+                  <c:v>308.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7915.0</c:v>
+                  <c:v>311.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16743.0</c:v>
+                  <c:v>334.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -544,11 +579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1982497440"/>
-        <c:axId val="-1988361664"/>
+        <c:axId val="-1980902416"/>
+        <c:axId val="-1990409600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1982497440"/>
+        <c:axId val="-1980902416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,12 +701,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988361664"/>
+        <c:crossAx val="-1990409600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1988361664"/>
+        <c:axId val="-1990409600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -778,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1982497440"/>
+        <c:crossAx val="-1980902416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1018,7 +1053,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>181.0</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,7 +1143,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>195.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,10 +1236,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>286.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>473.0</c:v>
+                  <c:v>141.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,7 +1329,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>683.0</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,10 +1422,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1380.0</c:v>
+                  <c:v>149.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3770.0</c:v>
+                  <c:v>308.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,7 +1515,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7915.0</c:v>
+                  <c:v>311.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1575,7 +1610,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>16743.0</c:v>
+                  <c:v>334.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,11 +1625,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1981962752"/>
-        <c:axId val="-1967628336"/>
+        <c:axId val="-2049335376"/>
+        <c:axId val="-2049496144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1981962752"/>
+        <c:axId val="-2049335376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,12 +1742,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1967628336"/>
+        <c:crossAx val="-2049496144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1967628336"/>
+        <c:axId val="-2049496144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1819,7 +1854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981962752"/>
+        <c:crossAx val="-2049335376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3312,10 +3347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3329,7 +3364,7 @@
     <col min="8" max="8" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3358,7 +3393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>125</v>
       </c>
@@ -3382,14 +3417,20 @@
         <v>1625</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <f>3*60+1</f>
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>125</v>
       </c>
@@ -3413,14 +3454,20 @@
         <v>3250</v>
       </c>
       <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5">
+        <v>70</v>
+      </c>
+      <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <f>3*60+15</f>
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>125</v>
       </c>
@@ -3444,14 +3491,20 @@
         <v>6500</v>
       </c>
       <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <f>4*60+46</f>
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>250</v>
       </c>
@@ -3475,14 +3528,20 @@
         <v>6500</v>
       </c>
       <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5">
+        <v>141</v>
+      </c>
+      <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <f>7*60+53</f>
         <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>250</v>
       </c>
@@ -3506,14 +3565,20 @@
         <v>13000</v>
       </c>
       <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="5">
+        <v>133</v>
+      </c>
+      <c r="K6" t="s">
         <v>11</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <f>11*60+23</f>
         <v>683</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>250</v>
       </c>
@@ -3537,14 +3602,20 @@
         <v>26000</v>
       </c>
       <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="5">
+        <v>149</v>
+      </c>
+      <c r="K7" t="s">
         <v>12</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <f>23*60</f>
         <v>1380</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>500</v>
       </c>
@@ -3568,14 +3639,21 @@
         <v>26000</v>
       </c>
       <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="5">
+        <f>5*60+8</f>
+        <v>308</v>
+      </c>
+      <c r="K8" t="s">
         <v>13</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <f>1*3600+2*60+50</f>
         <v>3770</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>500</v>
       </c>
@@ -3599,14 +3677,21 @@
         <v>52000</v>
       </c>
       <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="5">
+        <f>5*60+11</f>
+        <v>311</v>
+      </c>
+      <c r="K9" t="s">
         <v>14</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <f>2*3600+11*60+55</f>
         <v>7915</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>500</v>
       </c>
@@ -3630,18 +3715,352 @@
         <v>104000</v>
       </c>
       <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="5">
+        <f>5*60+34</f>
+        <v>334</v>
+      </c>
+      <c r="K10" t="s">
         <v>16</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <f>4*3600+39*60+3</f>
         <v>16743</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="G2" s="4">
+        <f>B2*D2*B2+C2*E2*B2+B2*F2*C2</f>
+        <v>1625</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G10" si="0">B3*D3*B3+C3*E3*B3+B3*F3*C3</f>
+        <v>3250</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>6500</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>250</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>6500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>250</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>13000</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>250</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>26000</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>500</v>
+      </c>
+      <c r="B8">
+        <v>400</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>26000</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="5">
+        <f>5*60+8</f>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>500</v>
+      </c>
+      <c r="B9">
+        <v>400</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>52000</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="5">
+        <f>5*60+11</f>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>500</v>
+      </c>
+      <c r="B10">
+        <v>400</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>104000</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="5">
+        <f>5*60+34</f>
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>